<commit_message>
separate dmbs from characters
characters from to dmbs
new characters model
</commit_message>
<xml_diff>
--- a/data/personajes.xlsx
+++ b/data/personajes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OdooCDev\custom\genshin_impact\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF6EBF-36F6-4297-B730-D48FB4799619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148BC759-7F81-4670-BDF1-C280C5EB1AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$L$48</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.42578125" defaultRowHeight="15"/>
@@ -621,16 +621,16 @@
         <v>53</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s">
         <v>65</v>
@@ -656,28 +656,28 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D3">
-        <v>82</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -688,19 +688,19 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D4">
         <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -720,13 +720,13 @@
         <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
         <v>65</v>
@@ -749,31 +749,31 @@
         <v>53</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="D6">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s">
         <v>65</v>
       </c>
       <c r="G6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -784,13 +784,13 @@
         <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
         <v>65</v>
@@ -816,13 +816,13 @@
         <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
@@ -848,13 +848,13 @@
         <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F9" t="s">
         <v>65</v>
@@ -877,31 +877,31 @@
         <v>53</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>55</v>
       </c>
       <c r="D10">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -912,16 +912,16 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -941,31 +941,31 @@
         <v>53</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="D12">
-        <v>80</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
         <v>66</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -973,31 +973,31 @@
         <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="D13">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1008,16 +1008,16 @@
         <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D14">
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -1037,31 +1037,31 @@
         <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="D15">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E15" t="s">
         <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1069,51 +1069,51 @@
         <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D16">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F16" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D17">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -1128,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -1136,16 +1136,16 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G18">
         <v>0</v>
@@ -1160,39 +1160,39 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
         <v>53</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="D19">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F19" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="G19">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H19">
         <v>1</v>
       </c>
       <c r="I19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -1200,77 +1200,77 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
+      <c r="A21" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+      <c r="E21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <v>20</v>
+      </c>
+      <c r="E22" t="s">
         <v>64</v>
-      </c>
-      <c r="F20" t="s">
-        <v>66</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>59</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>1</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-      <c r="J21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>88</v>
-      </c>
-      <c r="E22" t="s">
-        <v>60</v>
       </c>
       <c r="F22" t="s">
         <v>67</v>
@@ -1279,16 +1279,16 @@
         <v>1</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I22">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J22">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1296,32 +1296,31 @@
         <v>53</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="D23">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
         <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>6</v>
-      </c>
-      <c r="L23" s="1"/>
-    </row>
-    <row r="24" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1329,31 +1328,31 @@
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="D24">
-        <v>82</v>
+        <v>25</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G24">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I24">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J24">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1361,31 +1360,31 @@
         <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D25">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="E25" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25">
         <v>4</v>
       </c>
       <c r="J25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1393,127 +1392,127 @@
         <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D26">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="E26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27">
+        <v>40</v>
+      </c>
+      <c r="E27" t="s">
+        <v>64</v>
+      </c>
+      <c r="F27" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28">
+        <v>40</v>
+      </c>
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+      <c r="F28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
         <v>62</v>
       </c>
-      <c r="F26" t="s">
-        <v>67</v>
-      </c>
-      <c r="G26">
-        <v>3</v>
-      </c>
-      <c r="H26">
-        <v>4</v>
-      </c>
-      <c r="I26">
-        <v>8</v>
-      </c>
-      <c r="J26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C27" t="s">
-        <v>43</v>
-      </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>62</v>
-      </c>
-      <c r="F27" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27">
-        <v>0</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>1</v>
-      </c>
-      <c r="J27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28">
-        <v>90</v>
-      </c>
-      <c r="E28" t="s">
-        <v>64</v>
-      </c>
-      <c r="F28" t="s">
-        <v>67</v>
-      </c>
-      <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>6</v>
-      </c>
-      <c r="I28">
-        <v>7</v>
-      </c>
-      <c r="J28">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" t="s">
-        <v>53</v>
-      </c>
-      <c r="C29" t="s">
-        <v>26</v>
-      </c>
-      <c r="D29">
-        <v>20</v>
-      </c>
-      <c r="E29" t="s">
-        <v>64</v>
-      </c>
       <c r="F29" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1521,92 +1520,92 @@
         <v>53</v>
       </c>
       <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>63</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="s">
         <v>16</v>
       </c>
-      <c r="D30">
+      <c r="D31">
         <v>60</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E31" t="s">
         <v>59</v>
-      </c>
-      <c r="F30" t="s">
-        <v>68</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>4</v>
-      </c>
-      <c r="I30">
-        <v>6</v>
-      </c>
-      <c r="J30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12">
-      <c r="A31" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31" t="s">
-        <v>53</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31">
-        <v>20</v>
-      </c>
-      <c r="E31" t="s">
-        <v>60</v>
       </c>
       <c r="F31" t="s">
         <v>68</v>
       </c>
       <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32">
+        <v>70</v>
+      </c>
+      <c r="E32" t="s">
+        <v>61</v>
+      </c>
+      <c r="F32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>2</v>
       </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
       <c r="I32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J32">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:12">
@@ -1617,13 +1616,13 @@
         <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D33">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F33" t="s">
         <v>68</v>
@@ -1632,13 +1631,13 @@
         <v>0</v>
       </c>
       <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
         <v>2</v>
       </c>
-      <c r="I33">
+      <c r="J33">
         <v>4</v>
-      </c>
-      <c r="J33">
-        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:12">
@@ -1649,28 +1648,28 @@
         <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D34">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F34" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I34">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J34">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:12">
@@ -1678,31 +1677,31 @@
         <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>80</v>
       </c>
       <c r="E35" t="s">
         <v>62</v>
       </c>
       <c r="F35" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" spans="1:12">
@@ -1713,28 +1712,28 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D36">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="E36" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F36" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H36">
+        <v>3</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
         <v>6</v>
-      </c>
-      <c r="I36">
-        <v>8</v>
-      </c>
-      <c r="J36">
-        <v>11</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -1745,30 +1744,29 @@
         <v>53</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D37">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E37" t="s">
         <v>64</v>
       </c>
       <c r="F37" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I37">
         <v>5</v>
       </c>
       <c r="J37">
-        <v>6</v>
-      </c>
-      <c r="L37" s="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:12">
       <c r="A38" t="s">
@@ -1778,28 +1776,28 @@
         <v>53</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>82</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F38" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H38">
         <v>1</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J38">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:12">
@@ -1810,28 +1808,28 @@
         <v>53</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="D39">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="E39" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J39">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="40" spans="1:12">
@@ -1839,32 +1837,33 @@
         <v>53</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C40" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="E40" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F40" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G40">
         <v>0</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J40">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="L40" s="1"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" t="s">
@@ -1874,28 +1873,28 @@
         <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D41">
-        <v>25</v>
+        <v>85</v>
       </c>
       <c r="E41" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>2</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
       </c>
       <c r="I41">
         <v>4</v>
       </c>
       <c r="J41">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:12">
@@ -1903,64 +1902,66 @@
         <v>53</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="E42" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G42">
         <v>0</v>
       </c>
       <c r="H42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J42">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="L42" s="1"/>
     </row>
     <row r="43" spans="1:12">
       <c r="A43" t="s">
         <v>53</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="F43" t="s">
         <v>69</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J43">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="L43" s="1"/>
     </row>
     <row r="44" spans="1:12">
       <c r="A44" t="s">
@@ -1970,28 +1971,28 @@
         <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D44">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="F44" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44">
         <v>6</v>
       </c>
-      <c r="H44">
-        <v>3</v>
-      </c>
       <c r="I44">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J44">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="45" spans="1:12">
@@ -1999,31 +2000,31 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="E45" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J45">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="46" spans="1:12">
@@ -2031,31 +2032,31 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>1</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>90</v>
       </c>
       <c r="E46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F46" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I46">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J46">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -2066,30 +2067,29 @@
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D47">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E47" t="s">
         <v>63</v>
       </c>
       <c r="F47" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H47">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I47">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J47">
-        <v>9</v>
-      </c>
-      <c r="L47" s="1"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="48" spans="1:12">
       <c r="A48" t="s">
@@ -2099,36 +2099,32 @@
         <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="D48">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="E48" t="s">
         <v>64</v>
       </c>
       <c r="F48" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G48">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H48">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I48">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="J48">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L48">
-      <sortCondition ref="F1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:L48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>